<commit_message>
Added assumptions to supplemental calcs
</commit_message>
<xml_diff>
--- a/code/SludgeCosts.xlsx
+++ b/code/SludgeCosts.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27226"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28705"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="7120" yWindow="460" windowWidth="25360" windowHeight="16040" tabRatio="500"/>
+    <workbookView xWindow="6380" yWindow="2860" windowWidth="25600" windowHeight="15920" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="67">
   <si>
     <t>MGPY</t>
   </si>
@@ -151,6 +151,75 @@
   </si>
   <si>
     <t>$/ton</t>
+  </si>
+  <si>
+    <t>https://nepis.epa.gov/Exe/ZyNET.exe/P10053DP.txt?ZyActionD=ZyDocument&amp;Client=EPA&amp;Index=2000%20Thru%202005&amp;Docs=&amp;Query=%28cost%29%20OR%20FNAME%3D%22P10053DP.txt%22%20AND%20FNAME%3D%22P10053DP.txt%22&amp;Time=&amp;EndTime=&amp;SearchMethod=1&amp;TocRestrict=n&amp;Toc=&amp;TocEntry=&amp;QField=&amp;QFieldYear=&amp;QFieldMonth=&amp;QFieldDay=&amp;UseQField=&amp;IntQFieldOp=0&amp;ExtQFieldOp=0&amp;XmlQuery=&amp;File=D%3A%5CZYFILES%5CINDEX%20DATA%5C00THRU05%5CTXT%5C00000021%5CP10053DP.txt&amp;User=ANONYMOUS&amp;Password=anonymous&amp;SortMethod=h%7C-&amp;MaximumDocuments=1&amp;FuzzyDegree=0&amp;ImageQuality=r75g8/r75g8/x150y150g16/i425&amp;Display=hpfr&amp;DefSeekPage=x&amp;SearchBack=ZyActionL&amp;Back=ZyActionS&amp;BackDesc=Results%20page&amp;MaximumPages=1&amp;ZyEntry=7&amp;slide</t>
+  </si>
+  <si>
+    <t>$/Mg wet</t>
+  </si>
+  <si>
+    <t>% solids</t>
+  </si>
+  <si>
+    <t>$/Mg VSS landfilled</t>
+  </si>
+  <si>
+    <t>$/kg VSS landfilled</t>
+  </si>
+  <si>
+    <t>$/kg VSS Sent to Anaerobic Digester</t>
+  </si>
+  <si>
+    <t>Fraction of sludge reduced in AD</t>
+  </si>
+  <si>
+    <t>kgVSS</t>
+  </si>
+  <si>
+    <t>kgVSS to biogas</t>
+  </si>
+  <si>
+    <t>kgVSS to landfill</t>
+  </si>
+  <si>
+    <t>kg wet sludge to landfill</t>
+  </si>
+  <si>
+    <t>% biogas methane</t>
+  </si>
+  <si>
+    <t>gVSS/gCOD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cost to landfill 1kg sludge produced </t>
+  </si>
+  <si>
+    <t>kgCOD to biogas (as methane)</t>
+  </si>
+  <si>
+    <t>MJ/kg</t>
+  </si>
+  <si>
+    <t>MJ produced per 1 kg of sludge produced</t>
+  </si>
+  <si>
+    <t>kWh produced/1kg sludge</t>
+  </si>
+  <si>
+    <t>$/kWh of electricity, average US industrial</t>
+  </si>
+  <si>
+    <t>Metcalf&amp;Eddy</t>
+  </si>
+  <si>
+    <t>See supp calcs</t>
+  </si>
+  <si>
+    <t>https://www.eia.gov/electricity/monthly/epm_table_grapher.php?t=epmt_5_6_a</t>
+  </si>
+  <si>
+    <t>cost of energy recovered by WWTP</t>
   </si>
 </sst>
 </file>
@@ -211,7 +280,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="26">
+  <cellStyleXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -238,16 +307,24 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="9"/>
     <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="26">
+  <cellStyles count="31">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -268,6 +345,11 @@
     <cellStyle name="Followed Hyperlink" xfId="23" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="25" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="27" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="29" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -602,10 +684,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N21"/>
+  <dimension ref="A1:N39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="G39" sqref="G39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -899,7 +981,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="17" spans="8:11">
+    <row r="17" spans="6:11">
       <c r="I17" t="s">
         <v>36</v>
       </c>
@@ -907,7 +989,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="18" spans="8:11">
+    <row r="18" spans="6:11">
       <c r="H18" t="s">
         <v>41</v>
       </c>
@@ -921,7 +1003,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="19" spans="8:11">
+    <row r="19" spans="6:11">
       <c r="H19" t="s">
         <v>42</v>
       </c>
@@ -935,7 +1017,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="20" spans="8:11">
+    <row r="20" spans="6:11">
       <c r="I20">
         <f>I19/365*10^6</f>
         <v>19178.082191780824</v>
@@ -948,7 +1030,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="21" spans="8:11">
+    <row r="21" spans="6:11">
       <c r="I21" s="2">
         <f>I20/I18</f>
         <v>25.570776255707766</v>
@@ -959,6 +1041,174 @@
       </c>
       <c r="K21" t="s">
         <v>43</v>
+      </c>
+    </row>
+    <row r="30" spans="6:11">
+      <c r="F30">
+        <v>1</v>
+      </c>
+      <c r="G30" t="s">
+        <v>51</v>
+      </c>
+      <c r="I30">
+        <v>11</v>
+      </c>
+      <c r="J30" t="s">
+        <v>45</v>
+      </c>
+      <c r="K30" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="31" spans="6:11">
+      <c r="F31">
+        <f>I32*F30</f>
+        <v>0.59</v>
+      </c>
+      <c r="G31" t="s">
+        <v>52</v>
+      </c>
+      <c r="I31" s="6">
+        <f>AVERAGE(0.1,0.33)</f>
+        <v>0.21500000000000002</v>
+      </c>
+      <c r="J31" t="s">
+        <v>46</v>
+      </c>
+      <c r="K31" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="32" spans="6:11">
+      <c r="F32">
+        <f>F30-F31</f>
+        <v>0.41000000000000003</v>
+      </c>
+      <c r="G32" t="s">
+        <v>53</v>
+      </c>
+      <c r="H32" s="7"/>
+      <c r="I32" s="7">
+        <v>0.59</v>
+      </c>
+      <c r="J32" t="s">
+        <v>50</v>
+      </c>
+      <c r="K32" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="33" spans="6:12">
+      <c r="F33">
+        <f>F32/I31</f>
+        <v>1.9069767441860463</v>
+      </c>
+      <c r="G33" t="s">
+        <v>54</v>
+      </c>
+      <c r="I33">
+        <f>I30/I31</f>
+        <v>51.16279069767441</v>
+      </c>
+      <c r="J33" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="34" spans="6:12">
+      <c r="F34" s="5">
+        <f>F33/10^3*I30</f>
+        <v>2.097674418604651E-2</v>
+      </c>
+      <c r="G34" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="I34">
+        <f>I33/10^3</f>
+        <v>5.1162790697674411E-2</v>
+      </c>
+      <c r="J34" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="35" spans="6:12">
+      <c r="F35">
+        <f>F31/I37</f>
+        <v>0.39864864864864863</v>
+      </c>
+      <c r="G35" t="s">
+        <v>58</v>
+      </c>
+      <c r="I35">
+        <f>I34/I32</f>
+        <v>8.6716594402837993E-2</v>
+      </c>
+      <c r="J35" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="36" spans="6:12">
+      <c r="F36">
+        <f>F35*I38</f>
+        <v>21.925675675675674</v>
+      </c>
+      <c r="G36" t="s">
+        <v>60</v>
+      </c>
+      <c r="I36" s="6">
+        <v>0.62</v>
+      </c>
+      <c r="J36" t="s">
+        <v>55</v>
+      </c>
+      <c r="K36" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="37" spans="6:12">
+      <c r="F37">
+        <f>F36*10^6*0.0000002777778</f>
+        <v>6.0904659527027025</v>
+      </c>
+      <c r="G37" t="s">
+        <v>61</v>
+      </c>
+      <c r="I37">
+        <v>1.48</v>
+      </c>
+      <c r="J37" t="s">
+        <v>56</v>
+      </c>
+      <c r="K37" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="38" spans="6:12">
+      <c r="F38" s="5">
+        <f>F37*I39</f>
+        <v>0.42389643030810809</v>
+      </c>
+      <c r="G38" t="s">
+        <v>66</v>
+      </c>
+      <c r="I38">
+        <v>55</v>
+      </c>
+      <c r="J38" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="39" spans="6:12">
+      <c r="I39">
+        <v>6.9599999999999995E-2</v>
+      </c>
+      <c r="J39" t="s">
+        <v>62</v>
+      </c>
+      <c r="K39" s="8">
+        <v>43040</v>
+      </c>
+      <c r="L39" s="3" t="s">
+        <v>65</v>
       </c>
     </row>
   </sheetData>
@@ -969,6 +1219,7 @@
     <hyperlink ref="L15" r:id="rId4"/>
     <hyperlink ref="K16" r:id="rId5"/>
     <hyperlink ref="N15" r:id="rId6"/>
+    <hyperlink ref="L39" r:id="rId7"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>